<commit_message>
Actual Part Data Update for OM04
</commit_message>
<xml_diff>
--- a/FFR Data/Added Data/FFR Data Actual Part with Part code.xlsx
+++ b/FFR Data/Added Data/FFR Data Actual Part with Part code.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1474</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2977" uniqueCount="1534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3074" uniqueCount="1572">
   <si>
     <t>Actual Part</t>
   </si>
@@ -4624,6 +4625,120 @@
   </si>
   <si>
     <t>Valve</t>
+  </si>
+  <si>
+    <t>Fan Motor FW25K IR183GDR/SLK ODU</t>
+  </si>
+  <si>
+    <t>Blower SR183SG/SS IDU</t>
+  </si>
+  <si>
+    <t>Swing Louver SR183SG/SS IDU</t>
+  </si>
+  <si>
+    <t>Blower Motor BLDC SR183SG/SS IDU</t>
+  </si>
+  <si>
+    <t>Swing motor SR183SG/SS IDU</t>
+  </si>
+  <si>
+    <t>Main PCB SR183SG/SS IDU</t>
+  </si>
+  <si>
+    <t>COMPRESSOR (SHV33ZC1-S) S24TRDN2 ODU</t>
+  </si>
+  <si>
+    <t>4way Swing Motor MG Series IDU</t>
+  </si>
+  <si>
+    <t>Blower SR123SG/SS IDU</t>
+  </si>
+  <si>
+    <t>CONTROL PCB (5DF9) 18K3S4S/19K4S/24K3S IDU</t>
+  </si>
+  <si>
+    <t>Display pcb MG/MS/MB Series IDU</t>
+  </si>
+  <si>
+    <t>Blower Motor BLDC SR123SG/SS IDU</t>
+  </si>
+  <si>
+    <t>Main PCB SR123SG/SS IDU</t>
+  </si>
+  <si>
+    <t>Cam Link MG Series IDU</t>
+  </si>
+  <si>
+    <t>Display PCB SG/SS series IDU</t>
+  </si>
+  <si>
+    <t>FAN BLADE S09/12/18TRD4-G4-N4 ODU</t>
+  </si>
+  <si>
+    <t>CONTROL PCB (5EA1) 12K3S4S5S/18K5S IDU</t>
+  </si>
+  <si>
+    <t>TB Cover SR183SG/SS IDU</t>
+  </si>
+  <si>
+    <t>Evaporator Coil SR123SG/SS IDU</t>
+  </si>
+  <si>
+    <t>Swing motor SR123SG/SS IDU</t>
+  </si>
+  <si>
+    <t>BASE IR123/183GRD/IVR ODU</t>
+  </si>
+  <si>
+    <t>REACTOR INV12IRS/ONX ODU</t>
+  </si>
+  <si>
+    <t>SWING LOUVER HORZ IR183GNO IDU</t>
+  </si>
+  <si>
+    <t>Top Cover IR184/5/194TG/TS/MG/S/B ODU</t>
+  </si>
+  <si>
+    <t>CONTROL PCB (5270) IR194MB/MG/MS ODU</t>
+  </si>
+  <si>
+    <t>Evaporator Coil SR183SG/SS&amp;SR 193 SS/SG IDU</t>
+  </si>
+  <si>
+    <t>Display Cover Assy SR123/183SG/SS IDU</t>
+  </si>
+  <si>
+    <t>DisplaY PCB SR123/183AG IDU</t>
+  </si>
+  <si>
+    <t>Remote TG/TS/MG/MS/MB Series IDU</t>
+  </si>
+  <si>
+    <t>CONDENSOR ASSY SA093TRD ODU</t>
+  </si>
+  <si>
+    <t>CONTROL PCB ODU IR125URA</t>
+  </si>
+  <si>
+    <t>Part code</t>
+  </si>
+  <si>
+    <t>Part Name</t>
+  </si>
+  <si>
+    <t>Display Cover</t>
+  </si>
+  <si>
+    <t>ODU Top Cover</t>
+  </si>
+  <si>
+    <t>ODU Base</t>
+  </si>
+  <si>
+    <t>IDU Cam Link</t>
+  </si>
+  <si>
+    <t>Top Cover IDU</t>
   </si>
 </sst>
 </file>
@@ -4661,7 +4776,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -4684,11 +4799,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4718,6 +4848,13 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5024,16 +5161,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1506"/>
+  <dimension ref="A1:C1519"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1475" workbookViewId="0">
-      <selection activeCell="C1477" sqref="C1477"/>
+    <sheetView tabSelected="1" topLeftCell="A1503" workbookViewId="0">
+      <selection activeCell="B1519" sqref="B1519"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -21405,66 +21542,664 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="1489" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1489"/>
-    </row>
-    <row r="1490" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1490"/>
-    </row>
-    <row r="1491" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1491"/>
-    </row>
-    <row r="1492" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1492"/>
-    </row>
-    <row r="1493" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1493"/>
-    </row>
-    <row r="1494" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1494"/>
-    </row>
-    <row r="1495" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1495"/>
-    </row>
-    <row r="1496" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1496"/>
-    </row>
-    <row r="1497" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1497"/>
-    </row>
-    <row r="1498" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1498"/>
-    </row>
-    <row r="1499" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1499"/>
-    </row>
-    <row r="1500" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1500"/>
-    </row>
-    <row r="1501" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1501"/>
-    </row>
-    <row r="1502" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1502"/>
-    </row>
-    <row r="1503" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1503"/>
-    </row>
-    <row r="1504" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1504"/>
-    </row>
-    <row r="1505" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1505"/>
-    </row>
-    <row r="1506" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1506"/>
+    <row r="1489" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1489" s="12">
+        <v>11066407</v>
+      </c>
+      <c r="B1489" s="12" t="s">
+        <v>527</v>
+      </c>
+      <c r="C1489" s="12" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1490" s="12">
+        <v>11077052</v>
+      </c>
+      <c r="B1490" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1490" s="12" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1491" s="12">
+        <v>11077049</v>
+      </c>
+      <c r="B1491" s="12" t="s">
+        <v>530</v>
+      </c>
+      <c r="C1491" s="12" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1492" s="12">
+        <v>11077054</v>
+      </c>
+      <c r="B1492" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="C1492" s="12" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1493" s="12">
+        <v>11077064</v>
+      </c>
+      <c r="B1493" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="C1493" s="12" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1494" s="12">
+        <v>11077056</v>
+      </c>
+      <c r="B1494" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="C1494" s="12" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1495" s="12">
+        <v>11044381</v>
+      </c>
+      <c r="B1495" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="C1495" s="12" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1496" s="12">
+        <v>11077814</v>
+      </c>
+      <c r="B1496" s="12" t="s">
+        <v>524</v>
+      </c>
+      <c r="C1496" s="12" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1497" s="12">
+        <v>11077028</v>
+      </c>
+      <c r="B1497" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1497" s="12" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1498" s="12">
+        <v>11077847</v>
+      </c>
+      <c r="B1498" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="C1498" s="12" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1499" s="12">
+        <v>11077839</v>
+      </c>
+      <c r="B1499" s="12" t="s">
+        <v>521</v>
+      </c>
+      <c r="C1499" s="12" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1500" s="12">
+        <v>11077030</v>
+      </c>
+      <c r="B1500" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="C1500" s="12" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1501" s="12">
+        <v>11077032</v>
+      </c>
+      <c r="B1501" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="C1501" s="12" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1502" s="12">
+        <v>11077813</v>
+      </c>
+      <c r="B1502" s="12" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C1502" s="12" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="1503" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1503" s="12">
+        <v>11077042</v>
+      </c>
+      <c r="B1503" s="12" t="s">
+        <v>521</v>
+      </c>
+      <c r="C1503" s="12" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="1504" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1504" s="12">
+        <v>11048086</v>
+      </c>
+      <c r="B1504" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="C1504" s="12" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1505" s="12">
+        <v>11077846</v>
+      </c>
+      <c r="B1505" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="C1505" s="12" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1506" s="12">
+        <v>11077057</v>
+      </c>
+      <c r="B1506" s="12" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C1506" s="12" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1507" s="12">
+        <v>11077039</v>
+      </c>
+      <c r="B1507" s="12" t="s">
+        <v>519</v>
+      </c>
+      <c r="C1507" s="12" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1508" s="12">
+        <v>11077044</v>
+      </c>
+      <c r="B1508" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="C1508" s="12" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1509" s="12">
+        <v>11072513</v>
+      </c>
+      <c r="B1509" s="12" t="s">
+        <v>1569</v>
+      </c>
+      <c r="C1509" s="12" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1510" s="12">
+        <v>11060862</v>
+      </c>
+      <c r="B1510" s="12" t="s">
+        <v>540</v>
+      </c>
+      <c r="C1510" s="12" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1511" s="12">
+        <v>11065746</v>
+      </c>
+      <c r="B1511" s="12" t="s">
+        <v>530</v>
+      </c>
+      <c r="C1511" s="12" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1512" s="12">
+        <v>11077278</v>
+      </c>
+      <c r="B1512" s="12" t="s">
+        <v>1568</v>
+      </c>
+      <c r="C1512" s="12" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="1513" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1513" s="12">
+        <v>11077854</v>
+      </c>
+      <c r="B1513" s="12" t="s">
+        <v>520</v>
+      </c>
+      <c r="C1513" s="12" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1514" s="12">
+        <v>11077061</v>
+      </c>
+      <c r="B1514" s="12" t="s">
+        <v>519</v>
+      </c>
+      <c r="C1514" s="12" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="1515" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1515" s="12">
+        <v>11077041</v>
+      </c>
+      <c r="B1515" s="12" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C1515" s="12" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1516" s="12">
+        <v>11076636</v>
+      </c>
+      <c r="B1516" s="12" t="s">
+        <v>521</v>
+      </c>
+      <c r="C1516" s="12" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1517" s="12">
+        <v>11077263</v>
+      </c>
+      <c r="B1517" s="12" t="s">
+        <v>523</v>
+      </c>
+      <c r="C1517" s="12" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1518" s="12">
+        <v>11059270</v>
+      </c>
+      <c r="B1518" s="12" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1518" s="12" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1519" s="12">
+        <v>11068804</v>
+      </c>
+      <c r="B1519" s="12" t="s">
+        <v>520</v>
+      </c>
+      <c r="C1519" s="12" t="s">
+        <v>1564</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1488"/>
   <sortState ref="A2:C1071">
     <sortCondition ref="C2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>11066407</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>11077052</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>528</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>11077049</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>11077054</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>11077064</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>11077056</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>11044381</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>11077814</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>11077028</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>11077847</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>11077839</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>11077030</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>11077032</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>11077813</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>11077042</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>11048086</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>11077846</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>11077057</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>11077039</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>11077044</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>11072513</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>11060862</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>11065746</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>11077278</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>11077854</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>11077061</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>11077041</v>
+      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
+        <v>11076636</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>11077263</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>11059270</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
+        <v>11068804</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>